<commit_message>
Modify tests to pass before merging
</commit_message>
<xml_diff>
--- a/pattern_import_export_xlsx/tests/fixtures/example.users.fail.xlsx
+++ b/pattern_import_export_xlsx/tests/fixtures/example.users.fail.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t xml:space="preserve">YourCompany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ThatIdDoesntExist</t>
   </si>
   <si>
     <t xml:space="preserve">Mitchell Admin Updated</t>
@@ -143,10 +146,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.02"/>
   </cols>
@@ -174,11 +177,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
+      <c r="A3" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -212,7 +215,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>